<commit_message>
Riordinate e rinominate appropriatamente le ricerche locali sulla base della tesi
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/error_read_file.xlsx
+++ b/PS-VRP/Dati_output/error_read_file.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N202"/>
+  <dimension ref="A1:N102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,1007 +510,507 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>11</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>12</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>13</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>14</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>15</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>16</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>22</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>23</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>24</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>25</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>26</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>27</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>28</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>29</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>30</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>31</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>32</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>33</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>34</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>35</v>
+        <v>195</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>36</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>38</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>46</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>47</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>48</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>49</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>50</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>51</v>
+        <v>172</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>52</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>53</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>54</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>55</v>
+        <v>193</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>56</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>57</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>62</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>64</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>65</v>
+        <v>113</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>66</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>67</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>68</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>69</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>70</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>71</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>72</v>
+        <v>187</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>77</v>
+        <v>112</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>78</v>
+        <v>137</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>79</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>80</v>
+        <v>176</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>81</v>
+        <v>177</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>82</v>
+        <v>184</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>83</v>
+        <v>192</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>84</v>
+        <v>194</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>86</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>87</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>88</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>89</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>90</v>
+        <v>44</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>91</v>
+        <v>57</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>92</v>
+        <v>66</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>97</v>
+        <v>183</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>98</v>
+        <v>186</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>99</v>
+        <v>188</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="n">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="n">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="n">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="n">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="n">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="n">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="n">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="n">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="n">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="n">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="n">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="n">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="n">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="n">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="n">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="n">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="n">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="n">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="n">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="n">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="n">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="n">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="n">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="n">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="n">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="n">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="n">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="n">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="n">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="n">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="n">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="n">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="n">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="n">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="n">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="n">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="n">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="n">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="n">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="n">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="n">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="n">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="n">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="n">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="n">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="n">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="n">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="n">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="n">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="n">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="n">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="n">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="n">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="n">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="n">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="n">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="n">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="n">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="n">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="n">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="n">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="n">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="n">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="n">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="n">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="n">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="n">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="n">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="n">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="n">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="n">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="n">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="n">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="n">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="n">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="n">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" t="n">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" t="n">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" t="n">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" t="n">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="n">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="n">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" t="n">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" t="n">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" t="n">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" t="n">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" t="n">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" t="n">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="n">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="n">
         <v>196</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="n">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="n">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="n">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="n">
-        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Codice va ma problema coi dati
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/error_read_file.xlsx
+++ b/PS-VRP/Dati_output/error_read_file.xlsx
@@ -26,12 +26,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +52,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N102"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +451,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>data fine stampa</t>
+          <t>data fine stampa per schedulatore</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -509,508 +516,348 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
+      <c r="A2" s="1" t="n">
+        <v>233333</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>65</v>
+        <v>235572</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>125</v>
+        <v>243335</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>128</v>
+        <v>243569</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>129</v>
+        <v>244023</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>143</v>
+      <c r="A7" s="1" t="n">
+        <v>245623</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>147</v>
+        <v>250780</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>148</v>
+      <c r="A9" s="1" t="n">
+        <v>245089</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>152</v>
+        <v>251109</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>153</v>
+        <v>251129</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>155</v>
+        <v>251346</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>170</v>
+        <v>250344</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>174</v>
+        <v>251094</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>178</v>
+      <c r="A15" s="1" t="n">
+        <v>250497</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>179</v>
+      <c r="A16" s="1" t="n">
+        <v>251150</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>185</v>
+        <v>251100</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>200</v>
+        <v>251327</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>4</v>
+        <v>250866</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>17</v>
+      <c r="A20" s="1" t="n">
+        <v>250966</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
+      <c r="A21" s="1" t="n">
+        <v>250307</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>42</v>
+        <v>251281</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>43</v>
+        <v>250986</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>118</v>
+        <v>251402</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>122</v>
+      <c r="A25" s="1" t="n">
+        <v>251519</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>124</v>
+        <v>251522</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>130</v>
+      <c r="A27" s="1" t="n">
+        <v>251235</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>132</v>
+        <v>251550</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>134</v>
+      <c r="A29" s="1" t="n">
+        <v>250856</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>140</v>
+      <c r="A30" s="1" t="n">
+        <v>250855</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>145</v>
+      <c r="A31" s="1" t="n">
+        <v>251134</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>151</v>
+        <v>250208</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>168</v>
+        <v>250209</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>169</v>
+        <v>251250</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>171</v>
+        <v>251280</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>190</v>
+        <v>251088</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>195</v>
+        <v>251204</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>199</v>
+      <c r="A38" s="1" t="n">
+        <v>251015</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>11</v>
+        <v>251097</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>12</v>
+        <v>245413</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>18</v>
+      <c r="A41" s="1" t="n">
+        <v>250479</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>22</v>
+      <c r="A42" s="1" t="n">
+        <v>250478</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>39</v>
+        <v>251025</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>45</v>
+        <v>251033</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>47</v>
+      <c r="A45" s="1" t="n">
+        <v>250635</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>49</v>
+      <c r="A46" s="1" t="n">
+        <v>250637</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>54</v>
+      <c r="A47" s="1" t="n">
+        <v>251285</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>136</v>
+        <v>251442</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>138</v>
+        <v>251166</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>144</v>
+        <v>251427</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n">
-        <v>196</v>
+        <v>251614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prima implementazione secondo input reali
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/error_read_file.xlsx
+++ b/PS-VRP/Dati_output/error_read_file.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,12 +516,12 @@
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>Commesse::tassativita</t>
+          <t>flag tassativo taglio per schedulatore</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>Commesse::id_tassativo</t>
+          <t>id spedizione</t>
         </is>
       </c>
     </row>
@@ -539,6 +539,11 @@
           <t>CAMPO VUOTO</t>
         </is>
       </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
       <c r="P2" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
@@ -549,6 +554,11 @@
       <c r="A3" s="1" t="n">
         <v>235572</v>
       </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
       <c r="P3" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
@@ -559,6 +569,11 @@
       <c r="A4" s="1" t="n">
         <v>243335</v>
       </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
       <c r="P4" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
@@ -566,14 +581,29 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="n">
         <v>243569</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>244023</v>
       </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
       <c r="P6" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
@@ -589,6 +619,11 @@
           <t>CAMPO VUOTO</t>
         </is>
       </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
       <c r="P7" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
@@ -609,6 +644,11 @@
           <t>CAMPO VUOTO</t>
         </is>
       </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
       <c r="P9" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
@@ -624,6 +664,11 @@
           <t>CAMPO VUOTO</t>
         </is>
       </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
       <c r="P10" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
@@ -634,6 +679,11 @@
       <c r="A11" s="1" t="n">
         <v>251109</v>
       </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
       <c r="P11" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
@@ -649,6 +699,11 @@
           <t>CAMPO VUOTO</t>
         </is>
       </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
       <c r="P12" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
@@ -657,9 +712,9 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>251346</v>
-      </c>
-      <c r="P13" t="inlineStr">
+        <v>251211</v>
+      </c>
+      <c r="L13" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -667,9 +722,9 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>251519</v>
-      </c>
-      <c r="H14" t="inlineStr">
+        <v>251346</v>
+      </c>
+      <c r="O14" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -682,7 +737,17 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>251550</v>
+        <v>251519</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
@@ -691,25 +756,20 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>245275</v>
-      </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A16" t="n">
+        <v>250923</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>251310</v>
+        <v>251044</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="L17" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -717,9 +777,9 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>250819</v>
-      </c>
-      <c r="P18" t="inlineStr">
+        <v>250591</v>
+      </c>
+      <c r="L18" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -727,7 +787,12 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>251247</v>
+        <v>245275</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
@@ -736,35 +801,20 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>251317</v>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A20" t="n">
+        <v>251050</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>250913</v>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A21" t="n">
+        <v>251227</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>251846</v>
-      </c>
-      <c r="P22" t="inlineStr">
+        <v>251005</v>
+      </c>
+      <c r="L22" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -772,7 +822,17 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>251396</v>
+        <v>250918</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
@@ -782,7 +842,17 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>251455</v>
+        <v>251310</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
@@ -792,9 +862,9 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>251391</v>
-      </c>
-      <c r="P25" t="inlineStr">
+        <v>251081</v>
+      </c>
+      <c r="H25" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -802,9 +872,24 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>251651</v>
-      </c>
-      <c r="P26" t="inlineStr">
+        <v>251080</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -812,9 +897,24 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>251840</v>
-      </c>
-      <c r="P27" t="inlineStr">
+        <v>251079</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -822,9 +922,24 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>251458</v>
-      </c>
-      <c r="P28" t="inlineStr">
+        <v>251078</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -832,7 +947,12 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>251548</v>
+        <v>250819</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
@@ -842,7 +962,12 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>251547</v>
+        <v>251247</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
@@ -851,45 +976,30 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>251742</v>
-      </c>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A31" t="n">
+        <v>251225</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>251395</v>
-      </c>
-      <c r="P32" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A32" t="n">
+        <v>251421</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>251750</v>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A33" t="n">
+        <v>251268</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>251568</v>
-      </c>
-      <c r="P34" t="inlineStr">
+        <v>244960</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -897,32 +1007,32 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>251340</v>
+        <v>251371</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
       </c>
-      <c r="P35" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>251283</v>
-      </c>
-      <c r="P36" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A36" t="n">
+        <v>251782</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>251245</v>
+        <v>250913</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
@@ -932,7 +1042,12 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>251061</v>
+        <v>251846</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
@@ -941,80 +1056,40 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>251062</v>
-      </c>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A39" t="n">
+        <v>251477</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>251246</v>
-      </c>
-      <c r="P40" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A40" t="n">
+        <v>251054</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>245350</v>
-      </c>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A41" t="n">
+        <v>251396</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>251164</v>
-      </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A42" t="n">
+        <v>251453</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>250874</v>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A43" t="n">
+        <v>251455</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>251257</v>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A44" t="n">
+        <v>251391</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>251640</v>
-      </c>
-      <c r="I45" t="inlineStr">
+        <v>251651</v>
+      </c>
+      <c r="O45" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1026,78 +1101,38 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>251483</v>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P46" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A46" t="n">
+        <v>251840</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>251229</v>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A47" t="n">
+        <v>251548</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>251463</v>
-      </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A48" t="n">
+        <v>251547</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>251580</v>
-      </c>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A49" t="n">
+        <v>251742</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>251650</v>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
-      </c>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A50" t="n">
+        <v>251395</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>251416</v>
+        <v>251466</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
@@ -1107,7 +1142,17 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>250641</v>
+        <v>251750</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
@@ -1116,18 +1161,23 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>251464</v>
-      </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>CAMPO VUOTO</t>
-        </is>
+      <c r="A53" t="n">
+        <v>251456</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>251465</v>
+        <v>251340</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
@@ -1137,7 +1187,12 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>251462</v>
+        <v>251283</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
@@ -1147,7 +1202,12 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>251467</v>
+        <v>251245</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
@@ -1157,9 +1217,9 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>251795</v>
-      </c>
-      <c r="H57" t="inlineStr">
+        <v>251061</v>
+      </c>
+      <c r="O57" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>
@@ -1172,7 +1232,12 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>251284</v>
+        <v>251062</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
@@ -1182,7 +1247,12 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>251520</v>
+        <v>251246</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
@@ -1192,7 +1262,12 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>251986</v>
+        <v>245350</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
@@ -1201,10 +1276,805 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n">
+      <c r="A61" t="n">
+        <v>251164</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>250874</v>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>251257</v>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>251229</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>251463</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>251580</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>251650</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>251416</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>250641</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>251464</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P70" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>251465</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P71" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>251462</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>251467</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>251795</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P74" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>251284</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>251520</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
         <v>251987</v>
       </c>
-      <c r="P61" t="inlineStr">
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>251374</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>250894</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>251746</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>251585</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>251260</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>251373</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>244354</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>244355</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>251594</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>251743</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>251424</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>251397</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>244204</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>251561</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>251564</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>251809</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P93" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>251566</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P94" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>251626</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P95" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>251475</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P96" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>251761</v>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P97" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>251502</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P98" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>251706</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>251505</v>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P100" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>251557</v>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P101" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>251562</v>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P102" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>251546</v>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P103" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>250670</v>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P104" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>251485</v>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P105" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>251259</v>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P106" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>251252</v>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P107" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>251249</v>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P108" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>251251</v>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>CAMPO VUOTO</t>
+        </is>
+      </c>
+      <c r="P109" t="inlineStr">
         <is>
           <t>CAMPO VUOTO</t>
         </is>

</xml_diff>